<commit_message>
UPD INFO Toyota 20230421 1840
</commit_message>
<xml_diff>
--- a/TOYOTA-Celaya/Toyota - CEL - Analisis.xlsx
+++ b/TOYOTA-Celaya/Toyota - CEL - Analisis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KE\JMM\PROCESSES MAPPING\toyota_proceso\TOYOTA-Celaya\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D334BC38-21F0-43AA-8E4F-8EE00123843B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD219D8-D87B-492F-AE08-8289E53B601D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="0" windowWidth="19950" windowHeight="10800" activeTab="1" xr2:uid="{7E74557B-02A4-44EF-8F45-FC026D5565D6}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="335">
   <si>
     <t>Colaborador</t>
   </si>
@@ -1296,11 +1296,6 @@
 18:15 a 19:10 </t>
   </si>
   <si>
-    <t>Gina Mandujano
-( HYP ) 
-17:00 a 18:00</t>
-  </si>
-  <si>
     <t>Abr - 21</t>
   </si>
   <si>
@@ -1322,12 +1317,6 @@
 - Agendar Citas </t>
   </si>
   <si>
-    <t xml:space="preserve">Liz Mendoza
-( VDQ ) 
-12:00 a 14:00 
-</t>
-  </si>
-  <si>
     <t>Gina Mandujano
 ( HYP )
 08:30 a 10:00 
@@ -1337,17 +1326,6 @@
     <t xml:space="preserve">- Documentar 
 - Seguimientos  ( CALL )
 14:10 a 15:30  </t>
-  </si>
-  <si>
-    <t>Carlos Magueyal 
-( Jefe Taller ) 
-12:00 a ( 14:00 )  14:10 
-- Se comenzo de manera conjunta con Documentacion 
-- Se tuvieron interrupciones (tiempo) considerables imputables  a la Operacion.</t>
-  </si>
-  <si>
-    <t>- Documentar 
-18:30 a 19_</t>
   </si>
   <si>
     <t>Gaby Leones 
@@ -1364,7 +1342,47 @@
 08:30 a 11:30 </t>
   </si>
   <si>
-    <t>- Documentar</t>
+    <t>- Documentar 
+( GIT Push 11:58 )</t>
+  </si>
+  <si>
+    <t>Liz Mendoza
+( VDQ ) 
+12:00 a 14:30 
+Se presentaron algunas interrupciones por temas de la Operacion</t>
+  </si>
+  <si>
+    <t>Carlos Magueyal 
+( Jefe Taller ) 
+12:00 a ( 14:00 )  14:10 
+- Se comenzo de manera conjunta con Documentacion 
+- Se tuvieron interrupciones (tiempo) considerables por temas de la Operacion.</t>
+  </si>
+  <si>
+    <t>- Documentar 
+- Agendar 
+( Se agendo para el proximo Lunes una reunion con una colaboradora que hace Home Office y se encarga de las Asignaciones y Compras (se le conoce como Intercambios)</t>
+  </si>
+  <si>
+    <t>Teresa Navarrete 
+( Intercambios ) 
+15:30 - 17:00</t>
+  </si>
+  <si>
+    <t>Gina Mandujano
+( HYP ) 
+17:00 a 18:00 
+No se presento por temas de Operacion, entregaron un AUTO.
+- Se aprovecho para revisar con Marco Contreras los Avances de su Area incluidos colaboradores y la estrategia de seguimiento para la proxima semana.
+17:20 - 17:50</t>
+  </si>
+  <si>
+    <t>- Documentar 
+18:30 a 18:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Documentar 
+18:00 a </t>
   </si>
 </sst>
 </file>
@@ -1648,7 +1666,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1885,18 +1903,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1911,6 +1929,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2229,7 +2250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D791513-AAFD-400D-99BD-9246005A24E9}">
   <dimension ref="B2:J31"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -2843,8 +2864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643D6215-9EE1-49C2-914E-08742BC1E4A2}">
   <dimension ref="A2:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2854,8 +2875,8 @@
     <col min="3" max="3" width="36.42578125" style="57" customWidth="1"/>
     <col min="4" max="4" width="27.140625" style="57" customWidth="1"/>
     <col min="5" max="5" width="37.7109375" style="57" customWidth="1"/>
-    <col min="6" max="6" width="17" style="57" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="57" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" style="57" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="57" customWidth="1"/>
     <col min="8" max="15" width="9.140625" style="57"/>
     <col min="16" max="16" width="10.7109375" style="57" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="57"/>
@@ -2881,7 +2902,7 @@
     </row>
     <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="K3" s="58" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="54" customFormat="1" x14ac:dyDescent="0.25">
@@ -2896,7 +2917,7 @@
         <v>283</v>
       </c>
       <c r="F4" s="56" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G4" s="56" t="s">
         <v>289</v>
@@ -2937,10 +2958,10 @@
         <v>316</v>
       </c>
       <c r="E5" s="77" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F5" s="77" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="K5" s="59"/>
     </row>
@@ -2967,7 +2988,7 @@
         <v>304</v>
       </c>
       <c r="E7" s="64" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F7" s="77"/>
       <c r="K7" s="59"/>
@@ -2981,14 +3002,14 @@
         <v>312</v>
       </c>
       <c r="E8" s="70" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F8" s="65" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="K8" s="59"/>
     </row>
-    <row r="9" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="60" t="s">
         <v>278</v>
       </c>
@@ -2997,10 +3018,10 @@
       </c>
       <c r="D9" s="74"/>
       <c r="E9" s="77" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="F9" s="74" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="K9" s="59"/>
     </row>
@@ -3028,9 +3049,9 @@
       <c r="C11" s="75"/>
       <c r="D11" s="77"/>
       <c r="E11" s="59" t="s">
-        <v>326</v>
-      </c>
-      <c r="F11" s="59"/>
+        <v>324</v>
+      </c>
+      <c r="F11" s="74"/>
       <c r="G11" s="59"/>
       <c r="H11" s="59"/>
       <c r="I11" s="59"/>
@@ -3052,9 +3073,14 @@
         <v>314</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>329</v>
-      </c>
-      <c r="F12" s="68"/>
+        <v>325</v>
+      </c>
+      <c r="F12" s="65" t="s">
+        <v>330</v>
+      </c>
+      <c r="G12" s="77" t="s">
+        <v>331</v>
+      </c>
       <c r="K12" s="59"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -3067,9 +3093,10 @@
       </c>
       <c r="E13" s="72"/>
       <c r="F13" s="68"/>
+      <c r="G13" s="77"/>
       <c r="K13" s="59"/>
     </row>
-    <row r="14" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="165" x14ac:dyDescent="0.25">
       <c r="B14" s="60" t="s">
         <v>285</v>
       </c>
@@ -3079,7 +3106,7 @@
       <c r="D14" s="74"/>
       <c r="E14" s="72"/>
       <c r="F14" s="69" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="K14" s="59"/>
     </row>
@@ -3097,7 +3124,9 @@
         <v>318</v>
       </c>
       <c r="E15" s="72"/>
-      <c r="F15" s="59"/>
+      <c r="F15" s="89" t="s">
+        <v>334</v>
+      </c>
       <c r="G15" s="59"/>
       <c r="H15" s="59"/>
       <c r="I15" s="59"/>
@@ -3120,9 +3149,9 @@
       </c>
       <c r="D16" s="67"/>
       <c r="E16" s="67" t="s">
-        <v>328</v>
-      </c>
-      <c r="F16" s="67"/>
+        <v>333</v>
+      </c>
+      <c r="F16" s="89"/>
       <c r="G16" s="67"/>
       <c r="H16" s="67"/>
       <c r="I16" s="67"/>
@@ -3134,7 +3163,8 @@
       <c r="O16" s="67"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="F15:F16"/>
     <mergeCell ref="E12:E15"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="C12:C13"/>
@@ -3147,8 +3177,9 @@
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F9:F10"/>
     <mergeCell ref="F5:F7"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G12:G13"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3276,30 +3307,30 @@
       <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="I3" s="83" t="s">
+      <c r="I3" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="83" t="s">
+      <c r="N3" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="S3" s="82" t="s">
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="S3" s="81" t="s">
         <v>150</v>
       </c>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
@@ -3308,26 +3339,26 @@
       <c r="B5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="81" t="s">
+      <c r="D5" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="81"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="80"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="80"/>
+      <c r="T5" s="80"/>
+      <c r="U5" s="80"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
@@ -3336,16 +3367,16 @@
       <c r="B7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="81" t="s">
+      <c r="D7" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="81"/>
-      <c r="I7" s="81"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="81"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
@@ -3354,16 +3385,16 @@
       <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="81"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
@@ -3372,62 +3403,67 @@
       <c r="B11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="81" t="s">
+      <c r="D11" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="81"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="81"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="80"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="80"/>
+      <c r="P11" s="80"/>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="80" t="s">
+      <c r="I13" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="80"/>
-      <c r="K13" s="80"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="83"/>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="I15" s="80" t="s">
+      <c r="I15" s="83" t="s">
         <v>255</v>
       </c>
-      <c r="J15" s="80"/>
-      <c r="K15" s="80"/>
+      <c r="J15" s="83"/>
+      <c r="K15" s="83"/>
     </row>
     <row r="17" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I17" s="80" t="s">
+      <c r="I17" s="83" t="s">
         <v>256</v>
       </c>
-      <c r="J17" s="80"/>
-      <c r="K17" s="80"/>
+      <c r="J17" s="83"/>
+      <c r="K17" s="83"/>
     </row>
     <row r="19" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I19" s="80" t="s">
+      <c r="I19" s="83" t="s">
         <v>257</v>
       </c>
-      <c r="J19" s="80"/>
-      <c r="K19" s="80"/>
+      <c r="J19" s="83"/>
+      <c r="K19" s="83"/>
     </row>
     <row r="21" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I21" s="80" t="s">
+      <c r="I21" s="83" t="s">
         <v>258</v>
       </c>
-      <c r="J21" s="80"/>
-      <c r="K21" s="80"/>
+      <c r="J21" s="83"/>
+      <c r="K21" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I13:K13"/>
     <mergeCell ref="D7:K7"/>
     <mergeCell ref="D9:K9"/>
     <mergeCell ref="D11:P11"/>
@@ -3436,11 +3472,6 @@
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="I3:K3"/>
     <mergeCell ref="N3:P3"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I13:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>